<commit_message>
Adding within5 and closest columns to database, making more data persist
</commit_message>
<xml_diff>
--- a/app/tables/follow_arrival/forms/follow_arrival/follow_arrival.xlsx
+++ b/app/tables/follow_arrival/forms/follow_arrival/follow_arrival.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>clause</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>integer</t>
+  </si>
+  <si>
+    <t>FA_within_five_meters</t>
+  </si>
+  <si>
+    <t>Within 5 meters</t>
+  </si>
+  <si>
+    <t>FA_closest_to_focal</t>
+  </si>
+  <si>
+    <t>Closest to focal</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -709,14 +721,26 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="C12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="C13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="3"/>

</xml_diff>